<commit_message>
added append=TRUE to make new sheets in workbook
</commit_message>
<xml_diff>
--- a/alltogethernow.xlsx
+++ b/alltogethernow.xlsx
@@ -6,17 +6,75 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Raw" r:id="rId3" sheetId="1"/>
+    <sheet name="Counted" r:id="rId3" sheetId="1"/>
+    <sheet name="Raw" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="87">
   <si>
     <t>Failure_Reason</t>
   </si>
   <si>
+    <t>number_of_failures</t>
+  </si>
+  <si>
+    <t>-180</t>
+  </si>
+  <si>
+    <t>DMT on: TS</t>
+  </si>
+  <si>
+    <t>Dye contamination. 02/23/15 -APL</t>
+  </si>
+  <si>
+    <t>G-Rich Deprotection</t>
+  </si>
+  <si>
+    <t>MS not ok?low yield at ods sk 02/24/15</t>
+  </si>
+  <si>
+    <t>MS ok?low yield at ods 02/23/15 sd</t>
+  </si>
+  <si>
+    <t>MS ok: TS?low yield 2/24/2015 la</t>
+  </si>
+  <si>
+    <t>N-1 Failure</t>
+  </si>
+  <si>
+    <t>Poor BHQ3 coupling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor BHQ3 coupling </t>
+  </si>
+  <si>
+    <t>Purity</t>
+  </si>
+  <si>
+    <t>dye contamination. 02/24/15 -APL</t>
+  </si>
+  <si>
+    <t>poor synthesis: TS</t>
+  </si>
+  <si>
+    <t>see 336409 for syn. info. dw</t>
+  </si>
+  <si>
+    <t>see 336445 for syn. info. dw</t>
+  </si>
+  <si>
+    <t>see 336676 for syn. info. dw</t>
+  </si>
+  <si>
+    <t>wobble</t>
+  </si>
+  <si>
+    <t>wrong mass (-581): TS</t>
+  </si>
+  <si>
     <t>Five_Prime_mod</t>
   </si>
   <si>
@@ -24,60 +82,6 @@
   </si>
   <si>
     <t>sequence</t>
-  </si>
-  <si>
-    <t>-180</t>
-  </si>
-  <si>
-    <t>DMT on: TS</t>
-  </si>
-  <si>
-    <t>Dye contamination. 02/23/15 -APL</t>
-  </si>
-  <si>
-    <t>G-Rich Deprotection</t>
-  </si>
-  <si>
-    <t>MS not ok?low yield at ods sk 02/24/15</t>
-  </si>
-  <si>
-    <t>MS ok?low yield at ods 02/23/15 sd</t>
-  </si>
-  <si>
-    <t>MS ok: TS?low yield 2/24/2015 la</t>
-  </si>
-  <si>
-    <t>N-1 Failure</t>
-  </si>
-  <si>
-    <t>Poor BHQ3 coupling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poor BHQ3 coupling </t>
-  </si>
-  <si>
-    <t>Purity</t>
-  </si>
-  <si>
-    <t>dye contamination. 02/24/15 -APL</t>
-  </si>
-  <si>
-    <t>poor synthesis: TS</t>
-  </si>
-  <si>
-    <t>see 336409 for syn. info. dw</t>
-  </si>
-  <si>
-    <t>see 336445 for syn. info. dw</t>
-  </si>
-  <si>
-    <t>see 336676 for syn. info. dw</t>
-  </si>
-  <si>
-    <t>wobble</t>
-  </si>
-  <si>
-    <t>wrong mass (-581): TS</t>
   </si>
   <si>
     <t>BHQ-3</t>
@@ -327,268 +331,433 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>7.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
+      <c r="B4" t="n">
+        <v>9.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>9.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D15" t="s">
-        <v>47</v>
+        <v>15</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
+        <v>16</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
+        <v>17</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" t="e">
         <v>#N/A</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B20" t="e">
         <v>#N/A</v>
@@ -597,12 +766,12 @@
         <v>#N/A</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B21" t="e">
         <v>#N/A</v>
@@ -611,12 +780,12 @@
         <v>#N/A</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B22" t="e">
         <v>#N/A</v>
@@ -625,12 +794,12 @@
         <v>#N/A</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B23" t="e">
         <v>#N/A</v>
@@ -639,12 +808,12 @@
         <v>#N/A</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B24" t="e">
         <v>#N/A</v>
@@ -653,12 +822,12 @@
         <v>#N/A</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B25" t="e">
         <v>#N/A</v>
@@ -667,12 +836,12 @@
         <v>#N/A</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B26" t="e">
         <v>#N/A</v>
@@ -681,12 +850,12 @@
         <v>#N/A</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B27" t="e">
         <v>#N/A</v>
@@ -695,40 +864,40 @@
         <v>#N/A</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B28" t="e">
         <v>#N/A</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B29" t="e">
         <v>#N/A</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B30" t="e">
         <v>#N/A</v>
@@ -737,222 +906,222 @@
         <v>#N/A</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B31" t="e">
         <v>#N/A</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B32" t="e">
         <v>#N/A</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B33" t="e">
         <v>#N/A</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B34" t="e">
         <v>#N/A</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B35" t="e">
         <v>#N/A</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B36" t="e">
         <v>#N/A</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B37" t="e">
         <v>#N/A</v>
       </c>
       <c r="C37" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C38" t="e">
         <v>#N/A</v>
       </c>
       <c r="D38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C39" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C43" t="e">
         <v>#N/A</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C44" t="e">
         <v>#N/A</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C45" t="e">
         <v>#N/A</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B46" t="e">
         <v>#N/A</v>
@@ -961,12 +1130,12 @@
         <v>#N/A</v>
       </c>
       <c r="D46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B47" t="e">
         <v>#N/A</v>
@@ -975,12 +1144,12 @@
         <v>#N/A</v>
       </c>
       <c r="D47" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B48" t="e">
         <v>#N/A</v>
@@ -989,12 +1158,12 @@
         <v>#N/A</v>
       </c>
       <c r="D48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B49" t="e">
         <v>#N/A</v>
@@ -1003,12 +1172,12 @@
         <v>#N/A</v>
       </c>
       <c r="D49" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B50" t="e">
         <v>#N/A</v>
@@ -1017,12 +1186,12 @@
         <v>#N/A</v>
       </c>
       <c r="D50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B51" t="e">
         <v>#N/A</v>
@@ -1031,12 +1200,12 @@
         <v>#N/A</v>
       </c>
       <c r="D51" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B52" t="e">
         <v>#N/A</v>
@@ -1045,12 +1214,12 @@
         <v>#N/A</v>
       </c>
       <c r="D52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B53" t="e">
         <v>#N/A</v>
@@ -1059,12 +1228,12 @@
         <v>#N/A</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B54" t="e">
         <v>#N/A</v>
@@ -1073,54 +1242,54 @@
         <v>#N/A</v>
       </c>
       <c r="D54" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D55" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D56" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B58" t="e">
         <v>#N/A</v>
@@ -1129,12 +1298,12 @@
         <v>#N/A</v>
       </c>
       <c r="D58" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B59" t="e">
         <v>#N/A</v>
@@ -1143,12 +1312,12 @@
         <v>#N/A</v>
       </c>
       <c r="D59" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B60" t="e">
         <v>#N/A</v>
@@ -1157,21 +1326,21 @@
         <v>#N/A</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D61" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>